<commit_message>
Updated BoM with a cheaper connector from Newark
Todo:
*Create project documentation
</commit_message>
<xml_diff>
--- a/PCB Design/8 Cell Balancing Module/BoM.xlsx
+++ b/PCB Design/8 Cell Balancing Module/BoM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>Qty</t>
   </si>
@@ -167,28 +167,25 @@
     <t>Subtotal</t>
   </si>
   <si>
-    <t>Mouser</t>
-  </si>
-  <si>
-    <t>538-39500-0009</t>
-  </si>
-  <si>
-    <t>39500-0009</t>
-  </si>
-  <si>
-    <t>Molex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pluggable Terminal Blocks EURO 3.5MM HOR PLUG 9 CIRCUITS </t>
-  </si>
-  <si>
-    <t>538-39502-1009</t>
-  </si>
-  <si>
-    <t>39502-1009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pluggable Terminal Blocks 3.5MM HOR PCB HDR 9 CIRCUITS </t>
+    <t>Terminal Block Header, 9, 150 V, 12 A, 3.5 mm, Through Hole Right Angle, Header</t>
+  </si>
+  <si>
+    <t>MULTICOMP</t>
+  </si>
+  <si>
+    <t>54T7648</t>
+  </si>
+  <si>
+    <t>MCTE-03A09</t>
+  </si>
+  <si>
+    <t>Pluggable Terminal Block, 9, 3.5 mm, 24 AWG, 16 AWG</t>
+  </si>
+  <si>
+    <t>54T7625</t>
+  </si>
+  <si>
+    <t>MCTC-52A09</t>
   </si>
 </sst>
 </file>
@@ -548,8 +545,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,25 +806,25 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H9" s="11">
-        <v>2.66</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>31</v>
@@ -845,19 +842,19 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H10" s="11">
-        <v>3.28</v>
+        <v>1.27</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>45</v>
@@ -876,7 +873,7 @@
       </c>
       <c r="H12" s="11">
         <f>SUMPRODUCT(H2:H10,A2:A10)</f>
-        <v>18.468</v>
+        <v>14.571999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>